<commit_message>
se agrega campos en migraciones, en sus modelos, se arreglan importacion de consola y vista, se modifica excel para la carga
</commit_message>
<xml_diff>
--- a/public/imports/activos/plantilla_importar_activos.xlsx
+++ b/public/imports/activos/plantilla_importar_activos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\almacengt\public\imports\activos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9A2D81-4F0B-45BC-91E4-10A2EF6939C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAF5507-CB85-4A50-95BD-6FEBC0C7810E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E7B874D2-553A-4C08-A0F8-0EEE1A29FEDF}"/>
   </bookViews>
@@ -637,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14EDC99A-E6B0-432D-91FC-305AA62CA725}">
-  <dimension ref="A1:F1035"/>
+  <dimension ref="A1:G1035"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,12 +651,12 @@
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" style="4" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">

</xml_diff>